<commit_message>
Implementing edits to template page
Implementing edits to template page
</commit_message>
<xml_diff>
--- a/public/assets/Quantum_Health_Vendor_Template.xlsx
+++ b/public/assets/Quantum_Health_Vendor_Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sean.malone/Documents/CSV processor/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sean.malone/Documents/CSV new/react-drag-drop-csv-file/public/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{62A0CDDC-2215-D546-A5B1-3FC6B03D3F2B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4096E0D7-FF28-2845-98A4-CE79579F067E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,9 +23,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -135,6 +132,9 @@
   </si>
   <si>
     <t>Third-Party Administrator (TPA)</t>
+  </si>
+  <si>
+    <t>Vendor</t>
   </si>
 </sst>
 </file>
@@ -142,7 +142,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="\(###\)\ ###\-####"/>
+    <numFmt numFmtId="164" formatCode="\(###\)\ ###\-####"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -649,8 +649,8 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2"/>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1013,7 +1013,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1026,19 +1026,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
@@ -1070,167 +1070,167 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>